<commit_message>
feb 6 diary updated
</commit_message>
<xml_diff>
--- a/diaries/diary-Yijia-Zhang.xlsx
+++ b/diaries/diary-Yijia-Zhang.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Nice. Always feels good to have the homework done. </t>
   </si>
   <si>
-    <t>Class</t>
+    <t>Lecture</t>
   </si>
   <si>
     <t>Learnt about properties of mental models. Refresher on UML diagram. Filled forms for feature discovery.</t>
@@ -200,6 +200,58 @@
   </si>
   <si>
     <t>:D</t>
+  </si>
+  <si>
+    <t>Unfortunately could not attend  lecture due to personal issues. Awaiting the slides.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="12"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Missing a 3-hour lecture really hurts :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <t>:((((</t>
+  </si>
+  <si>
+    <t>Find essential features</t>
+  </si>
+  <si>
+    <t>Found them quite easily</t>
+  </si>
+  <si>
+    <t>One thing good about choosing an application for inspection is that we can derive feature from program specifications and according to its usage. In our case, our program of choice was Telegram, the instant messaging app. Then message sending is easily selected as essential feature.</t>
+  </si>
+  <si>
+    <t>Go over the slides</t>
+  </si>
+  <si>
+    <t>Went over last lecture’s slides</t>
+  </si>
+  <si>
+    <t>Gotta attend the lecture</t>
+  </si>
+  <si>
+    <t>A new template (of thought process) was introduced. Listened to a very experienced engineer’s talk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The template was a bit weird compared to previous ones, at least in terms of column naming. But I can see it helps with tracing how essential variables are manipulated by functions, giving better organized comprehension of program (feature) functionality. </t>
+  </si>
+  <si>
+    <t>Being able to attend again feels great. Unfortunately I was not told to bring a printed copy of dairy. Again shows how much I’d miss not being able to attend a lecture. I would like to suggest, though, that maybe we can have assignments and important requirements listed on the course web page if possible. (Thank you)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +262,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -288,6 +340,16 @@
       <b val="1"/>
       <i val="1"/>
       <sz val="12"/>
+      <color indexed="15"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="15"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="15"/>
       <name val="Helvetica"/>
     </font>
@@ -419,7 +481,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -513,17 +575,32 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -1900,985 +1977,1023 @@
       </c>
     </row>
     <row r="17" ht="93.25" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" ht="15.5" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-    </row>
-    <row r="19" ht="15.5" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-    </row>
-    <row r="20" ht="15.5" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="A17" s="27">
+        <v>43860</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" t="s" s="33">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s" s="20">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" ht="75.95" customHeight="1">
+      <c r="A18" s="27">
+        <v>43863</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" t="s" s="35">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s" s="20">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s" s="20">
+        <v>56</v>
+      </c>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" ht="91.25" customHeight="1">
+      <c r="A19" s="27">
+        <v>43865</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" t="s" s="21">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s" s="33">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s" s="20">
+        <v>59</v>
+      </c>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="20" ht="152" customHeight="1">
+      <c r="A20" s="27">
+        <v>43867</v>
+      </c>
+      <c r="B20" t="s" s="20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s" s="37">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s" s="20">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s" s="21">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="33"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="33"/>
+      <c r="A46" s="38"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="33"/>
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="33"/>
+      <c r="A48" s="38"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
+      <c r="A49" s="38"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="31"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="33"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="31"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
+      <c r="A52" s="38"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="31"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="33"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="31"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="36"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="31"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
+      <c r="A55" s="38"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="36"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="33"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="31"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="33"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="36"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="33"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="33"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="33"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="36"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="33"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="33"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="33"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="31"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="33"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="31"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="33"/>
+      <c r="A66" s="38"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="33"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="36"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="31"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="33"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="36"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="31"/>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="31"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="36"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="33"/>
+      <c r="A71" s="38"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="36"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="33"/>
+      <c r="A72" s="38"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="33"/>
+      <c r="A73" s="38"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="36"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="33"/>
+      <c r="A74" s="38"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="36"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="33"/>
+      <c r="A75" s="38"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="31"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33"/>
+      <c r="A76" s="38"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="31"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="33"/>
+      <c r="A77" s="38"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="31"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="33"/>
+      <c r="A78" s="38"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="33"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="36"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="31"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="33"/>
+      <c r="A80" s="38"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="33"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="33"/>
+      <c r="A82" s="38"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="33"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="36"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="31"/>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="33"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="36"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="31"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="33"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="36"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="31"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="33"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="36"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="33"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="36"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="31"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="33"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="36"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="31"/>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="32"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="33"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="31"/>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="33"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="36"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="31"/>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="33"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="36"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="31"/>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="36"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="31"/>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="33"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="36"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="31"/>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="33"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="36"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="31"/>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="33"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39"/>
+      <c r="G95" s="36"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="31"/>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="33"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="39"/>
+      <c r="G96" s="36"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="31"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="33"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
+      <c r="E97" s="39"/>
+      <c r="F97" s="39"/>
+      <c r="G97" s="36"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="31"/>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="32"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="33"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="39"/>
+      <c r="C98" s="39"/>
+      <c r="D98" s="39"/>
+      <c r="E98" s="39"/>
+      <c r="F98" s="39"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="31"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="32"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="33"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39"/>
+      <c r="G99" s="36"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="31"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="32"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="33"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="39"/>
+      <c r="D100" s="39"/>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39"/>
+      <c r="G100" s="36"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="31"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="33"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
+      <c r="E101" s="39"/>
+      <c r="F101" s="39"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="31"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="33"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="36"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="31"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="33"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
+      <c r="E103" s="39"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="36"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="31"/>
-      <c r="B104" s="32"/>
-      <c r="C104" s="32"/>
-      <c r="D104" s="32"/>
-      <c r="E104" s="32"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="33"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="39"/>
+      <c r="C104" s="39"/>
+      <c r="D104" s="39"/>
+      <c r="E104" s="39"/>
+      <c r="F104" s="39"/>
+      <c r="G104" s="36"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="31"/>
-      <c r="B105" s="32"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
-      <c r="E105" s="32"/>
-      <c r="F105" s="32"/>
-      <c r="G105" s="33"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="39"/>
+      <c r="C105" s="39"/>
+      <c r="D105" s="39"/>
+      <c r="E105" s="39"/>
+      <c r="F105" s="39"/>
+      <c r="G105" s="36"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="31"/>
-      <c r="B106" s="32"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="32"/>
-      <c r="G106" s="33"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="39"/>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="36"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="31"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="33"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="39"/>
+      <c r="D107" s="39"/>
+      <c r="E107" s="39"/>
+      <c r="F107" s="39"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="31"/>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32"/>
-      <c r="E108" s="32"/>
-      <c r="F108" s="32"/>
-      <c r="G108" s="33"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="39"/>
+      <c r="C108" s="39"/>
+      <c r="D108" s="39"/>
+      <c r="E108" s="39"/>
+      <c r="F108" s="39"/>
+      <c r="G108" s="36"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="31"/>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="32"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="33"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="39"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39"/>
+      <c r="G109" s="36"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="31"/>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="33"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="39"/>
+      <c r="C110" s="39"/>
+      <c r="D110" s="39"/>
+      <c r="E110" s="39"/>
+      <c r="F110" s="39"/>
+      <c r="G110" s="36"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="31"/>
-      <c r="B111" s="32"/>
-      <c r="C111" s="32"/>
-      <c r="D111" s="32"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="32"/>
-      <c r="G111" s="33"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="39"/>
+      <c r="G111" s="36"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="31"/>
-      <c r="B112" s="32"/>
-      <c r="C112" s="32"/>
-      <c r="D112" s="32"/>
-      <c r="E112" s="32"/>
-      <c r="F112" s="32"/>
-      <c r="G112" s="33"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="39"/>
+      <c r="C112" s="39"/>
+      <c r="D112" s="39"/>
+      <c r="E112" s="39"/>
+      <c r="F112" s="39"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="31"/>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="33"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="36"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="31"/>
-      <c r="B114" s="32"/>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="33"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="39"/>
+      <c r="D114" s="39"/>
+      <c r="E114" s="39"/>
+      <c r="F114" s="39"/>
+      <c r="G114" s="36"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="31"/>
-      <c r="B115" s="32"/>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="32"/>
-      <c r="F115" s="32"/>
-      <c r="G115" s="33"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="39"/>
+      <c r="E115" s="39"/>
+      <c r="F115" s="39"/>
+      <c r="G115" s="36"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="31"/>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32"/>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="33"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="39"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="39"/>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39"/>
+      <c r="G116" s="36"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="31"/>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32"/>
-      <c r="D117" s="32"/>
-      <c r="E117" s="32"/>
-      <c r="F117" s="32"/>
-      <c r="G117" s="33"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="39"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="39"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="36"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="31"/>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32"/>
-      <c r="D118" s="32"/>
-      <c r="E118" s="32"/>
-      <c r="F118" s="32"/>
-      <c r="G118" s="33"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="39"/>
+      <c r="C118" s="39"/>
+      <c r="D118" s="39"/>
+      <c r="E118" s="39"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="36"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="31"/>
-      <c r="B119" s="32"/>
-      <c r="C119" s="32"/>
-      <c r="D119" s="32"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="32"/>
-      <c r="G119" s="33"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="36"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="31"/>
-      <c r="B120" s="32"/>
-      <c r="C120" s="32"/>
-      <c r="D120" s="32"/>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="33"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="39"/>
+      <c r="C120" s="39"/>
+      <c r="D120" s="39"/>
+      <c r="E120" s="39"/>
+      <c r="F120" s="39"/>
+      <c r="G120" s="36"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="31"/>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32"/>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="33"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="39"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="39"/>
+      <c r="E121" s="39"/>
+      <c r="F121" s="39"/>
+      <c r="G121" s="36"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="31"/>
-      <c r="B122" s="32"/>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="33"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
+      <c r="F122" s="39"/>
+      <c r="G122" s="36"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="31"/>
-      <c r="B123" s="32"/>
-      <c r="C123" s="32"/>
-      <c r="D123" s="32"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32"/>
-      <c r="G123" s="33"/>
+      <c r="A123" s="38"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="39"/>
+      <c r="E123" s="39"/>
+      <c r="F123" s="39"/>
+      <c r="G123" s="36"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="31"/>
-      <c r="B124" s="32"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="32"/>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32"/>
-      <c r="G124" s="33"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="39"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="39"/>
+      <c r="E124" s="39"/>
+      <c r="F124" s="39"/>
+      <c r="G124" s="36"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="36"/>
-      <c r="B125" s="37"/>
-      <c r="C125" s="37"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="38"/>
+      <c r="A125" s="41"/>
+      <c r="B125" s="42"/>
+      <c r="C125" s="42"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="42"/>
+      <c r="F125" s="42"/>
+      <c r="G125" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Yijia Zhang Dec.6 diary updated (DS_Store removed) (#299)
* feb 6 diary updated

* Delete .DS_Store
</commit_message>
<xml_diff>
--- a/diaries/diary-Yijia-Zhang.xlsx
+++ b/diaries/diary-Yijia-Zhang.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Nice. Always feels good to have the homework done. </t>
   </si>
   <si>
-    <t>Class</t>
+    <t>Lecture</t>
   </si>
   <si>
     <t>Learnt about properties of mental models. Refresher on UML diagram. Filled forms for feature discovery.</t>
@@ -200,6 +200,58 @@
   </si>
   <si>
     <t>:D</t>
+  </si>
+  <si>
+    <t>Unfortunately could not attend  lecture due to personal issues. Awaiting the slides.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="12"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Missing a 3-hour lecture really hurts :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <t>:((((</t>
+  </si>
+  <si>
+    <t>Find essential features</t>
+  </si>
+  <si>
+    <t>Found them quite easily</t>
+  </si>
+  <si>
+    <t>One thing good about choosing an application for inspection is that we can derive feature from program specifications and according to its usage. In our case, our program of choice was Telegram, the instant messaging app. Then message sending is easily selected as essential feature.</t>
+  </si>
+  <si>
+    <t>Go over the slides</t>
+  </si>
+  <si>
+    <t>Went over last lecture’s slides</t>
+  </si>
+  <si>
+    <t>Gotta attend the lecture</t>
+  </si>
+  <si>
+    <t>A new template (of thought process) was introduced. Listened to a very experienced engineer’s talk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The template was a bit weird compared to previous ones, at least in terms of column naming. But I can see it helps with tracing how essential variables are manipulated by functions, giving better organized comprehension of program (feature) functionality. </t>
+  </si>
+  <si>
+    <t>Being able to attend again feels great. Unfortunately I was not told to bring a printed copy of dairy. Again shows how much I’d miss not being able to attend a lecture. I would like to suggest, though, that maybe we can have assignments and important requirements listed on the course web page if possible. (Thank you)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +262,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -288,6 +340,16 @@
       <b val="1"/>
       <i val="1"/>
       <sz val="12"/>
+      <color indexed="15"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="15"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="15"/>
       <name val="Helvetica"/>
     </font>
@@ -419,7 +481,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -513,17 +575,32 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -1900,985 +1977,1023 @@
       </c>
     </row>
     <row r="17" ht="93.25" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" ht="15.5" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-    </row>
-    <row r="19" ht="15.5" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-    </row>
-    <row r="20" ht="15.5" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="A17" s="27">
+        <v>43860</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" t="s" s="33">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s" s="20">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" ht="75.95" customHeight="1">
+      <c r="A18" s="27">
+        <v>43863</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" t="s" s="35">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s" s="20">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s" s="20">
+        <v>56</v>
+      </c>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" ht="91.25" customHeight="1">
+      <c r="A19" s="27">
+        <v>43865</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" t="s" s="21">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s" s="33">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s" s="20">
+        <v>59</v>
+      </c>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="20" ht="152" customHeight="1">
+      <c r="A20" s="27">
+        <v>43867</v>
+      </c>
+      <c r="B20" t="s" s="20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s" s="37">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s" s="20">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="G20" t="s" s="21">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="33"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="33"/>
+      <c r="A46" s="38"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="33"/>
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="33"/>
+      <c r="A48" s="38"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
+      <c r="A49" s="38"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="31"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="33"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="31"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
+      <c r="A52" s="38"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="31"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="33"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="31"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="36"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="31"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
+      <c r="A55" s="38"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="36"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="33"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="31"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="33"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="36"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="33"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="33"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="33"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="36"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="33"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="33"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="33"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="31"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="33"/>
+      <c r="A65" s="38"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="31"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="33"/>
+      <c r="A66" s="38"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="33"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="36"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="31"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="33"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="36"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="31"/>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="31"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
+      <c r="A70" s="38"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="36"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="33"/>
+      <c r="A71" s="38"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="36"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="33"/>
+      <c r="A72" s="38"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="33"/>
+      <c r="A73" s="38"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="36"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="33"/>
+      <c r="A74" s="38"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="36"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="33"/>
+      <c r="A75" s="38"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="31"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33"/>
+      <c r="A76" s="38"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="31"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="33"/>
+      <c r="A77" s="38"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="31"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="33"/>
+      <c r="A78" s="38"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="33"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="36"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="31"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="33"/>
+      <c r="A80" s="38"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="33"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="33"/>
+      <c r="A82" s="38"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="33"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="36"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="31"/>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
-      <c r="E84" s="32"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="33"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="36"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="31"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="33"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="36"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="31"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="33"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="36"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="33"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="36"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="31"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="33"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="36"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="31"/>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="32"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="33"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="31"/>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="33"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="36"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="31"/>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="33"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="36"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="31"/>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="36"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="31"/>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="33"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="36"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="31"/>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="33"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="36"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="31"/>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="33"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39"/>
+      <c r="G95" s="36"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="31"/>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="33"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="39"/>
+      <c r="G96" s="36"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="31"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="33"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
+      <c r="E97" s="39"/>
+      <c r="F97" s="39"/>
+      <c r="G97" s="36"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="31"/>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="32"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="33"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="39"/>
+      <c r="C98" s="39"/>
+      <c r="D98" s="39"/>
+      <c r="E98" s="39"/>
+      <c r="F98" s="39"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="31"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="32"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="33"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39"/>
+      <c r="G99" s="36"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="31"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="32"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="33"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="39"/>
+      <c r="D100" s="39"/>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39"/>
+      <c r="G100" s="36"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="31"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="33"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
+      <c r="E101" s="39"/>
+      <c r="F101" s="39"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="31"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="33"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="36"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="31"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="33"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
+      <c r="E103" s="39"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="36"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="31"/>
-      <c r="B104" s="32"/>
-      <c r="C104" s="32"/>
-      <c r="D104" s="32"/>
-      <c r="E104" s="32"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="33"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="39"/>
+      <c r="C104" s="39"/>
+      <c r="D104" s="39"/>
+      <c r="E104" s="39"/>
+      <c r="F104" s="39"/>
+      <c r="G104" s="36"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="31"/>
-      <c r="B105" s="32"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
-      <c r="E105" s="32"/>
-      <c r="F105" s="32"/>
-      <c r="G105" s="33"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="39"/>
+      <c r="C105" s="39"/>
+      <c r="D105" s="39"/>
+      <c r="E105" s="39"/>
+      <c r="F105" s="39"/>
+      <c r="G105" s="36"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="31"/>
-      <c r="B106" s="32"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="32"/>
-      <c r="G106" s="33"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="39"/>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="36"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="31"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="33"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="39"/>
+      <c r="D107" s="39"/>
+      <c r="E107" s="39"/>
+      <c r="F107" s="39"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="31"/>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32"/>
-      <c r="E108" s="32"/>
-      <c r="F108" s="32"/>
-      <c r="G108" s="33"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="39"/>
+      <c r="C108" s="39"/>
+      <c r="D108" s="39"/>
+      <c r="E108" s="39"/>
+      <c r="F108" s="39"/>
+      <c r="G108" s="36"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="31"/>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="32"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="33"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="39"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39"/>
+      <c r="G109" s="36"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="31"/>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="33"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="39"/>
+      <c r="C110" s="39"/>
+      <c r="D110" s="39"/>
+      <c r="E110" s="39"/>
+      <c r="F110" s="39"/>
+      <c r="G110" s="36"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="31"/>
-      <c r="B111" s="32"/>
-      <c r="C111" s="32"/>
-      <c r="D111" s="32"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="32"/>
-      <c r="G111" s="33"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="39"/>
+      <c r="G111" s="36"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="31"/>
-      <c r="B112" s="32"/>
-      <c r="C112" s="32"/>
-      <c r="D112" s="32"/>
-      <c r="E112" s="32"/>
-      <c r="F112" s="32"/>
-      <c r="G112" s="33"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="39"/>
+      <c r="C112" s="39"/>
+      <c r="D112" s="39"/>
+      <c r="E112" s="39"/>
+      <c r="F112" s="39"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="31"/>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="33"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="36"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="31"/>
-      <c r="B114" s="32"/>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="33"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="39"/>
+      <c r="D114" s="39"/>
+      <c r="E114" s="39"/>
+      <c r="F114" s="39"/>
+      <c r="G114" s="36"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="31"/>
-      <c r="B115" s="32"/>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="32"/>
-      <c r="F115" s="32"/>
-      <c r="G115" s="33"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="39"/>
+      <c r="E115" s="39"/>
+      <c r="F115" s="39"/>
+      <c r="G115" s="36"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="31"/>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32"/>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="33"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="39"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="39"/>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39"/>
+      <c r="G116" s="36"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="31"/>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32"/>
-      <c r="D117" s="32"/>
-      <c r="E117" s="32"/>
-      <c r="F117" s="32"/>
-      <c r="G117" s="33"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="39"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="39"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="36"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="31"/>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32"/>
-      <c r="D118" s="32"/>
-      <c r="E118" s="32"/>
-      <c r="F118" s="32"/>
-      <c r="G118" s="33"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="39"/>
+      <c r="C118" s="39"/>
+      <c r="D118" s="39"/>
+      <c r="E118" s="39"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="36"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="31"/>
-      <c r="B119" s="32"/>
-      <c r="C119" s="32"/>
-      <c r="D119" s="32"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="32"/>
-      <c r="G119" s="33"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="36"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="31"/>
-      <c r="B120" s="32"/>
-      <c r="C120" s="32"/>
-      <c r="D120" s="32"/>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="33"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="39"/>
+      <c r="C120" s="39"/>
+      <c r="D120" s="39"/>
+      <c r="E120" s="39"/>
+      <c r="F120" s="39"/>
+      <c r="G120" s="36"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="31"/>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32"/>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="33"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="39"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="39"/>
+      <c r="E121" s="39"/>
+      <c r="F121" s="39"/>
+      <c r="G121" s="36"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="31"/>
-      <c r="B122" s="32"/>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="33"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
+      <c r="F122" s="39"/>
+      <c r="G122" s="36"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="31"/>
-      <c r="B123" s="32"/>
-      <c r="C123" s="32"/>
-      <c r="D123" s="32"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32"/>
-      <c r="G123" s="33"/>
+      <c r="A123" s="38"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="39"/>
+      <c r="E123" s="39"/>
+      <c r="F123" s="39"/>
+      <c r="G123" s="36"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="31"/>
-      <c r="B124" s="32"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="32"/>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32"/>
-      <c r="G124" s="33"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="39"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="39"/>
+      <c r="E124" s="39"/>
+      <c r="F124" s="39"/>
+      <c r="G124" s="36"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">
-      <c r="A125" s="36"/>
-      <c r="B125" s="37"/>
-      <c r="C125" s="37"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="38"/>
+      <c r="A125" s="41"/>
+      <c r="B125" s="42"/>
+      <c r="C125" s="42"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="42"/>
+      <c r="F125" s="42"/>
+      <c r="G125" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Recent diary updated Yijia Zhang (#402)
* feb 6 diary updated

* Delete .DS_Store

* recent diaries updated
</commit_message>
<xml_diff>
--- a/diaries/diary-Yijia-Zhang.xlsx
+++ b/diaries/diary-Yijia-Zhang.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -253,14 +253,78 @@
   <si>
     <t>Being able to attend again feels great. Unfortunately I was not told to bring a printed copy of dairy. Again shows how much I’d miss not being able to attend a lecture. I would like to suggest, though, that maybe we can have assignments and important requirements listed on the course web page if possible. (Thank you)</t>
   </si>
+  <si>
+    <t xml:space="preserve">21:00 - 2.12 ??? </t>
+  </si>
+  <si>
+    <t>Study for midterm</t>
+  </si>
+  <si>
+    <t>Reviewed the slides, refreshed memory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got to review the slides more often in the future, as many details/concepts gets easily forgotten over time. It’s extra trouble trying to pick them back up. </t>
+  </si>
+  <si>
+    <t>THE MIDTERM IS BACK UHHHHH</t>
+  </si>
+  <si>
+    <t>Survive the Midterm</t>
+  </si>
+  <si>
+    <t>Barely finished the midterm. Quickly went through this week’s material.</t>
+  </si>
+  <si>
+    <t>Haven’t been able to write quickly since I had never written anything in around half a year… Feeling sincerely sorry for Kaj for having to try to read my handwriting. Feels okay about the exam, as there were no multiple choice problems. Could not really focus afterward. Will review the slides at home.</t>
+  </si>
+  <si>
+    <t>Not sure… Depends on the midterm score.</t>
+  </si>
+  <si>
+    <t>20:00-?</t>
+  </si>
+  <si>
+    <t>Review last week’s slides</t>
+  </si>
+  <si>
+    <t>Went through the slides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should have focused in class </t>
+  </si>
+  <si>
+    <t>:(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learnt about concepts and methods toward Architectural recovery. </t>
+  </si>
+  <si>
+    <t>Contents today reminds me of the concept “architectural drift” that I learnt in 264P at the beginning of the quarter. The guest speakers were informative and fun. Both (of course) agrees on that separation of concerns is vitally important. Also one should try to write short methods, as having short methods shows that one has thought about and can control his structure and style of code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive. </t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Score was out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe I didn’t study hard enough?  Not sure what costed my 6 points… </t>
+  </si>
+  <si>
+    <t>Depressed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="60" formatCode="m/d"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -596,13 +660,13 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="60" fontId="11" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2050,940 +2114,1008 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" ht="15.5" customHeight="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="36"/>
-    </row>
-    <row r="22" ht="15.5" customHeight="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="36"/>
-    </row>
-    <row r="23" ht="15.5" customHeight="1">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="36"/>
-    </row>
-    <row r="24" ht="15.5" customHeight="1">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="36"/>
-    </row>
-    <row r="25" ht="15.5" customHeight="1">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="36"/>
-    </row>
-    <row r="26" ht="15.5" customHeight="1">
-      <c r="A26" s="38"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+    <row r="21" ht="152.6" customHeight="1">
+      <c r="A21" s="38">
+        <v>43872</v>
+      </c>
+      <c r="B21" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s" s="37">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s" s="20">
+        <v>66</v>
+      </c>
+      <c r="G21" t="s" s="21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" ht="162.85" customHeight="1">
+      <c r="A22" s="38">
+        <v>43874</v>
+      </c>
+      <c r="B22" t="s" s="20">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s" s="20">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s" s="20">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s" s="20">
+        <v>70</v>
+      </c>
+      <c r="G22" t="s" s="21">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" ht="91.15" customHeight="1">
+      <c r="A23" s="38">
+        <v>43880</v>
+      </c>
+      <c r="B23" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s" s="20">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="F23" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s" s="21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" ht="204.1" customHeight="1">
+      <c r="A24" s="38">
+        <v>43881</v>
+      </c>
+      <c r="B24" t="s" s="20">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s" s="20">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s" s="20">
+        <v>77</v>
+      </c>
+      <c r="F24" t="s" s="20">
+        <v>78</v>
+      </c>
+      <c r="G24" t="s" s="21">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" ht="106.2" customHeight="1">
+      <c r="A25" s="38">
+        <v>43885</v>
+      </c>
+      <c r="B25" t="s" s="20">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" t="s" s="20">
+        <v>81</v>
+      </c>
+      <c r="F25" t="s" s="20">
+        <v>82</v>
+      </c>
+      <c r="G25" t="s" s="21">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" ht="104.45" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
       <c r="G26" s="36"/>
     </row>
     <row r="27" ht="15.5" customHeight="1">
-      <c r="A27" s="38"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
       <c r="G27" s="36"/>
     </row>
     <row r="28" ht="15.5" customHeight="1">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="36"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="36"/>
     </row>
     <row r="30" ht="15.5" customHeight="1">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
       <c r="G30" s="36"/>
     </row>
     <row r="31" ht="15.5" customHeight="1">
-      <c r="A31" s="38"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
       <c r="G31" s="36"/>
     </row>
     <row r="32" ht="15.5" customHeight="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
       <c r="G32" s="36"/>
     </row>
     <row r="33" ht="15.5" customHeight="1">
-      <c r="A33" s="38"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="36"/>
     </row>
     <row r="34" ht="15.5" customHeight="1">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="36"/>
     </row>
     <row r="35" ht="15.5" customHeight="1">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="36"/>
     </row>
     <row r="36" ht="15.5" customHeight="1">
-      <c r="A36" s="38"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="36"/>
     </row>
     <row r="37" ht="15.5" customHeight="1">
-      <c r="A37" s="38"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="36"/>
     </row>
     <row r="38" ht="15.5" customHeight="1">
-      <c r="A38" s="38"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
       <c r="G38" s="36"/>
     </row>
     <row r="39" ht="15.5" customHeight="1">
-      <c r="A39" s="38"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
       <c r="G39" s="36"/>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
       <c r="G40" s="36"/>
     </row>
     <row r="41" ht="15.5" customHeight="1">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
       <c r="G41" s="36"/>
     </row>
     <row r="42" ht="15.5" customHeight="1">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
       <c r="G42" s="36"/>
     </row>
     <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="36"/>
     </row>
     <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="38"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
       <c r="G44" s="36"/>
     </row>
     <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
       <c r="G45" s="36"/>
     </row>
     <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="38"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
       <c r="G46" s="36"/>
     </row>
     <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="38"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
       <c r="G47" s="36"/>
     </row>
     <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="38"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
       <c r="G48" s="36"/>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="38"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
       <c r="G49" s="36"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
       <c r="G50" s="36"/>
     </row>
     <row r="51" ht="15.5" customHeight="1">
-      <c r="A51" s="38"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
       <c r="G51" s="36"/>
     </row>
     <row r="52" ht="15.5" customHeight="1">
-      <c r="A52" s="38"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
       <c r="G52" s="36"/>
     </row>
     <row r="53" ht="15.5" customHeight="1">
-      <c r="A53" s="38"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
       <c r="G53" s="36"/>
     </row>
     <row r="54" ht="15.5" customHeight="1">
-      <c r="A54" s="38"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
       <c r="G54" s="36"/>
     </row>
     <row r="55" ht="15.5" customHeight="1">
-      <c r="A55" s="38"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
       <c r="G55" s="36"/>
     </row>
     <row r="56" ht="15.5" customHeight="1">
-      <c r="A56" s="38"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
       <c r="G56" s="36"/>
     </row>
     <row r="57" ht="15.5" customHeight="1">
-      <c r="A57" s="38"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
       <c r="G57" s="36"/>
     </row>
     <row r="58" ht="15.5" customHeight="1">
-      <c r="A58" s="38"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
       <c r="G58" s="36"/>
     </row>
     <row r="59" ht="15.5" customHeight="1">
-      <c r="A59" s="38"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
       <c r="G59" s="36"/>
     </row>
     <row r="60" ht="15.5" customHeight="1">
-      <c r="A60" s="38"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
       <c r="G60" s="36"/>
     </row>
     <row r="61" ht="15.5" customHeight="1">
-      <c r="A61" s="38"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
       <c r="G61" s="36"/>
     </row>
     <row r="62" ht="15.5" customHeight="1">
-      <c r="A62" s="38"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
       <c r="G62" s="36"/>
     </row>
     <row r="63" ht="15.5" customHeight="1">
-      <c r="A63" s="38"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
       <c r="G63" s="36"/>
     </row>
     <row r="64" ht="15.5" customHeight="1">
-      <c r="A64" s="38"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
       <c r="G64" s="36"/>
     </row>
     <row r="65" ht="15.5" customHeight="1">
-      <c r="A65" s="38"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
+      <c r="A65" s="39"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
       <c r="G65" s="36"/>
     </row>
     <row r="66" ht="15.5" customHeight="1">
-      <c r="A66" s="38"/>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
       <c r="G66" s="36"/>
     </row>
     <row r="67" ht="15.5" customHeight="1">
-      <c r="A67" s="38"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
       <c r="G67" s="36"/>
     </row>
     <row r="68" ht="15.5" customHeight="1">
-      <c r="A68" s="38"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
       <c r="G68" s="36"/>
     </row>
     <row r="69" ht="15.5" customHeight="1">
-      <c r="A69" s="38"/>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
       <c r="G69" s="36"/>
     </row>
     <row r="70" ht="15.5" customHeight="1">
-      <c r="A70" s="38"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="40"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="40"/>
       <c r="G70" s="36"/>
     </row>
     <row r="71" ht="15.5" customHeight="1">
-      <c r="A71" s="38"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
       <c r="G71" s="36"/>
     </row>
     <row r="72" ht="15.5" customHeight="1">
-      <c r="A72" s="38"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
       <c r="G72" s="36"/>
     </row>
     <row r="73" ht="15.5" customHeight="1">
-      <c r="A73" s="38"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="40"/>
+      <c r="F73" s="40"/>
       <c r="G73" s="36"/>
     </row>
     <row r="74" ht="15.5" customHeight="1">
-      <c r="A74" s="38"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="40"/>
+      <c r="F74" s="40"/>
       <c r="G74" s="36"/>
     </row>
     <row r="75" ht="15.5" customHeight="1">
-      <c r="A75" s="38"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
+      <c r="A75" s="39"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="40"/>
       <c r="G75" s="36"/>
     </row>
     <row r="76" ht="15.5" customHeight="1">
-      <c r="A76" s="38"/>
-      <c r="B76" s="39"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
       <c r="G76" s="36"/>
     </row>
     <row r="77" ht="15.5" customHeight="1">
-      <c r="A77" s="38"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="40"/>
+      <c r="F77" s="40"/>
       <c r="G77" s="36"/>
     </row>
     <row r="78" ht="15.5" customHeight="1">
-      <c r="A78" s="38"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+      <c r="F78" s="40"/>
       <c r="G78" s="36"/>
     </row>
     <row r="79" ht="15.5" customHeight="1">
-      <c r="A79" s="38"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="39"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="40"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
+      <c r="F79" s="40"/>
       <c r="G79" s="36"/>
     </row>
     <row r="80" ht="15.5" customHeight="1">
-      <c r="A80" s="38"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="39"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
+      <c r="D80" s="40"/>
+      <c r="E80" s="40"/>
+      <c r="F80" s="40"/>
       <c r="G80" s="36"/>
     </row>
     <row r="81" ht="15.5" customHeight="1">
-      <c r="A81" s="38"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
-      <c r="F81" s="39"/>
+      <c r="A81" s="39"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="40"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="40"/>
+      <c r="F81" s="40"/>
       <c r="G81" s="36"/>
     </row>
     <row r="82" ht="15.5" customHeight="1">
-      <c r="A82" s="38"/>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="39"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="40"/>
+      <c r="F82" s="40"/>
       <c r="G82" s="36"/>
     </row>
     <row r="83" ht="15.5" customHeight="1">
-      <c r="A83" s="38"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="40"/>
+      <c r="F83" s="40"/>
       <c r="G83" s="36"/>
     </row>
     <row r="84" ht="15.5" customHeight="1">
-      <c r="A84" s="38"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
+      <c r="A84" s="39"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="40"/>
+      <c r="F84" s="40"/>
       <c r="G84" s="36"/>
     </row>
     <row r="85" ht="15.5" customHeight="1">
-      <c r="A85" s="38"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="39"/>
+      <c r="A85" s="39"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="40"/>
+      <c r="F85" s="40"/>
       <c r="G85" s="36"/>
     </row>
     <row r="86" ht="15.5" customHeight="1">
-      <c r="A86" s="38"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="39"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="40"/>
+      <c r="F86" s="40"/>
       <c r="G86" s="36"/>
     </row>
     <row r="87" ht="15.5" customHeight="1">
-      <c r="A87" s="38"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
+      <c r="A87" s="39"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="40"/>
+      <c r="F87" s="40"/>
       <c r="G87" s="36"/>
     </row>
     <row r="88" ht="15.5" customHeight="1">
-      <c r="A88" s="38"/>
-      <c r="B88" s="39"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
+      <c r="A88" s="39"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="40"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="40"/>
+      <c r="F88" s="40"/>
       <c r="G88" s="36"/>
     </row>
     <row r="89" ht="15.5" customHeight="1">
-      <c r="A89" s="38"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
+      <c r="A89" s="39"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
+      <c r="D89" s="40"/>
+      <c r="E89" s="40"/>
+      <c r="F89" s="40"/>
       <c r="G89" s="36"/>
     </row>
     <row r="90" ht="15.5" customHeight="1">
-      <c r="A90" s="38"/>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
+      <c r="A90" s="39"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="40"/>
+      <c r="D90" s="40"/>
+      <c r="E90" s="40"/>
+      <c r="F90" s="40"/>
       <c r="G90" s="36"/>
     </row>
     <row r="91" ht="15.5" customHeight="1">
-      <c r="A91" s="38"/>
-      <c r="B91" s="39"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
-      <c r="F91" s="39"/>
+      <c r="A91" s="39"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="40"/>
+      <c r="D91" s="40"/>
+      <c r="E91" s="40"/>
+      <c r="F91" s="40"/>
       <c r="G91" s="36"/>
     </row>
     <row r="92" ht="15.5" customHeight="1">
-      <c r="A92" s="38"/>
-      <c r="B92" s="39"/>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
-      <c r="F92" s="39"/>
+      <c r="A92" s="39"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="40"/>
+      <c r="F92" s="40"/>
       <c r="G92" s="36"/>
     </row>
     <row r="93" ht="15.5" customHeight="1">
-      <c r="A93" s="38"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
+      <c r="A93" s="39"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="40"/>
+      <c r="F93" s="40"/>
       <c r="G93" s="36"/>
     </row>
     <row r="94" ht="15.5" customHeight="1">
-      <c r="A94" s="38"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
+      <c r="A94" s="39"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
+      <c r="E94" s="40"/>
+      <c r="F94" s="40"/>
       <c r="G94" s="36"/>
     </row>
     <row r="95" ht="15.5" customHeight="1">
-      <c r="A95" s="38"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
+      <c r="A95" s="39"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="40"/>
+      <c r="F95" s="40"/>
       <c r="G95" s="36"/>
     </row>
     <row r="96" ht="15.5" customHeight="1">
-      <c r="A96" s="38"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
-      <c r="F96" s="39"/>
+      <c r="A96" s="39"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="40"/>
+      <c r="F96" s="40"/>
       <c r="G96" s="36"/>
     </row>
     <row r="97" ht="15.5" customHeight="1">
-      <c r="A97" s="38"/>
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
-      <c r="F97" s="39"/>
+      <c r="A97" s="39"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="40"/>
+      <c r="F97" s="40"/>
       <c r="G97" s="36"/>
     </row>
     <row r="98" ht="15.5" customHeight="1">
-      <c r="A98" s="38"/>
-      <c r="B98" s="39"/>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
+      <c r="A98" s="39"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="40"/>
+      <c r="D98" s="40"/>
+      <c r="E98" s="40"/>
+      <c r="F98" s="40"/>
       <c r="G98" s="36"/>
     </row>
     <row r="99" ht="15.5" customHeight="1">
-      <c r="A99" s="38"/>
-      <c r="B99" s="39"/>
-      <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="39"/>
-      <c r="F99" s="39"/>
+      <c r="A99" s="39"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="40"/>
+      <c r="F99" s="40"/>
       <c r="G99" s="36"/>
     </row>
     <row r="100" ht="15.5" customHeight="1">
-      <c r="A100" s="38"/>
-      <c r="B100" s="39"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
+      <c r="A100" s="39"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="40"/>
+      <c r="D100" s="40"/>
+      <c r="E100" s="40"/>
+      <c r="F100" s="40"/>
       <c r="G100" s="36"/>
     </row>
     <row r="101" ht="15.5" customHeight="1">
-      <c r="A101" s="38"/>
-      <c r="B101" s="39"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
+      <c r="A101" s="39"/>
+      <c r="B101" s="40"/>
+      <c r="C101" s="40"/>
+      <c r="D101" s="40"/>
+      <c r="E101" s="40"/>
+      <c r="F101" s="40"/>
       <c r="G101" s="36"/>
     </row>
     <row r="102" ht="15.5" customHeight="1">
-      <c r="A102" s="38"/>
-      <c r="B102" s="39"/>
-      <c r="C102" s="39"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
-      <c r="F102" s="39"/>
+      <c r="A102" s="39"/>
+      <c r="B102" s="40"/>
+      <c r="C102" s="40"/>
+      <c r="D102" s="40"/>
+      <c r="E102" s="40"/>
+      <c r="F102" s="40"/>
       <c r="G102" s="36"/>
     </row>
     <row r="103" ht="15.5" customHeight="1">
-      <c r="A103" s="38"/>
-      <c r="B103" s="39"/>
-      <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
-      <c r="F103" s="39"/>
+      <c r="A103" s="39"/>
+      <c r="B103" s="40"/>
+      <c r="C103" s="40"/>
+      <c r="D103" s="40"/>
+      <c r="E103" s="40"/>
+      <c r="F103" s="40"/>
       <c r="G103" s="36"/>
     </row>
     <row r="104" ht="15.5" customHeight="1">
-      <c r="A104" s="38"/>
-      <c r="B104" s="39"/>
-      <c r="C104" s="39"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
-      <c r="F104" s="39"/>
+      <c r="A104" s="39"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="40"/>
+      <c r="D104" s="40"/>
+      <c r="E104" s="40"/>
+      <c r="F104" s="40"/>
       <c r="G104" s="36"/>
     </row>
     <row r="105" ht="15.5" customHeight="1">
-      <c r="A105" s="38"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
-      <c r="F105" s="39"/>
+      <c r="A105" s="39"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="40"/>
+      <c r="E105" s="40"/>
+      <c r="F105" s="40"/>
       <c r="G105" s="36"/>
     </row>
     <row r="106" ht="15.5" customHeight="1">
-      <c r="A106" s="38"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
+      <c r="A106" s="39"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="40"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="40"/>
+      <c r="F106" s="40"/>
       <c r="G106" s="36"/>
     </row>
     <row r="107" ht="15.5" customHeight="1">
-      <c r="A107" s="38"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="39"/>
-      <c r="E107" s="39"/>
-      <c r="F107" s="39"/>
+      <c r="A107" s="39"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="40"/>
+      <c r="D107" s="40"/>
+      <c r="E107" s="40"/>
+      <c r="F107" s="40"/>
       <c r="G107" s="36"/>
     </row>
     <row r="108" ht="15.5" customHeight="1">
-      <c r="A108" s="38"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
+      <c r="A108" s="39"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="40"/>
+      <c r="D108" s="40"/>
+      <c r="E108" s="40"/>
+      <c r="F108" s="40"/>
       <c r="G108" s="36"/>
     </row>
     <row r="109" ht="15.5" customHeight="1">
-      <c r="A109" s="38"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
+      <c r="A109" s="39"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
+      <c r="E109" s="40"/>
+      <c r="F109" s="40"/>
       <c r="G109" s="36"/>
     </row>
     <row r="110" ht="15.5" customHeight="1">
-      <c r="A110" s="38"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="39"/>
-      <c r="F110" s="39"/>
+      <c r="A110" s="39"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="40"/>
+      <c r="D110" s="40"/>
+      <c r="E110" s="40"/>
+      <c r="F110" s="40"/>
       <c r="G110" s="36"/>
     </row>
     <row r="111" ht="15.5" customHeight="1">
-      <c r="A111" s="38"/>
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
-      <c r="F111" s="39"/>
+      <c r="A111" s="39"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="40"/>
+      <c r="D111" s="40"/>
+      <c r="E111" s="40"/>
+      <c r="F111" s="40"/>
       <c r="G111" s="36"/>
     </row>
     <row r="112" ht="15.5" customHeight="1">
-      <c r="A112" s="38"/>
-      <c r="B112" s="39"/>
-      <c r="C112" s="39"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
-      <c r="F112" s="39"/>
+      <c r="A112" s="39"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="40"/>
+      <c r="D112" s="40"/>
+      <c r="E112" s="40"/>
+      <c r="F112" s="40"/>
       <c r="G112" s="36"/>
     </row>
     <row r="113" ht="15.5" customHeight="1">
-      <c r="A113" s="38"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
-      <c r="F113" s="39"/>
+      <c r="A113" s="39"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="40"/>
+      <c r="D113" s="40"/>
+      <c r="E113" s="40"/>
+      <c r="F113" s="40"/>
       <c r="G113" s="36"/>
     </row>
     <row r="114" ht="15.5" customHeight="1">
-      <c r="A114" s="38"/>
-      <c r="B114" s="39"/>
-      <c r="C114" s="39"/>
-      <c r="D114" s="39"/>
-      <c r="E114" s="39"/>
-      <c r="F114" s="39"/>
+      <c r="A114" s="39"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="40"/>
+      <c r="D114" s="40"/>
+      <c r="E114" s="40"/>
+      <c r="F114" s="40"/>
       <c r="G114" s="36"/>
     </row>
     <row r="115" ht="15.5" customHeight="1">
-      <c r="A115" s="38"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="39"/>
-      <c r="F115" s="39"/>
+      <c r="A115" s="39"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="40"/>
+      <c r="D115" s="40"/>
+      <c r="E115" s="40"/>
+      <c r="F115" s="40"/>
       <c r="G115" s="36"/>
     </row>
     <row r="116" ht="15.5" customHeight="1">
-      <c r="A116" s="38"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
-      <c r="F116" s="39"/>
+      <c r="A116" s="39"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
+      <c r="E116" s="40"/>
+      <c r="F116" s="40"/>
       <c r="G116" s="36"/>
     </row>
     <row r="117" ht="15.5" customHeight="1">
-      <c r="A117" s="38"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="39"/>
-      <c r="F117" s="39"/>
+      <c r="A117" s="39"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
+      <c r="D117" s="40"/>
+      <c r="E117" s="40"/>
+      <c r="F117" s="40"/>
       <c r="G117" s="36"/>
     </row>
     <row r="118" ht="15.5" customHeight="1">
-      <c r="A118" s="38"/>
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="39"/>
-      <c r="F118" s="39"/>
+      <c r="A118" s="39"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="40"/>
+      <c r="D118" s="40"/>
+      <c r="E118" s="40"/>
+      <c r="F118" s="40"/>
       <c r="G118" s="36"/>
     </row>
     <row r="119" ht="15.5" customHeight="1">
-      <c r="A119" s="38"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
+      <c r="A119" s="39"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
+      <c r="E119" s="40"/>
+      <c r="F119" s="40"/>
       <c r="G119" s="36"/>
     </row>
     <row r="120" ht="15.5" customHeight="1">
-      <c r="A120" s="38"/>
-      <c r="B120" s="39"/>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="39"/>
-      <c r="F120" s="39"/>
+      <c r="A120" s="39"/>
+      <c r="B120" s="40"/>
+      <c r="C120" s="40"/>
+      <c r="D120" s="40"/>
+      <c r="E120" s="40"/>
+      <c r="F120" s="40"/>
       <c r="G120" s="36"/>
     </row>
     <row r="121" ht="15.5" customHeight="1">
-      <c r="A121" s="38"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="39"/>
-      <c r="F121" s="39"/>
+      <c r="A121" s="39"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
+      <c r="E121" s="40"/>
+      <c r="F121" s="40"/>
       <c r="G121" s="36"/>
     </row>
     <row r="122" ht="15.5" customHeight="1">
-      <c r="A122" s="38"/>
-      <c r="B122" s="39"/>
-      <c r="C122" s="39"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="39"/>
-      <c r="F122" s="39"/>
+      <c r="A122" s="39"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
+      <c r="E122" s="40"/>
+      <c r="F122" s="40"/>
       <c r="G122" s="36"/>
     </row>
     <row r="123" ht="15.5" customHeight="1">
-      <c r="A123" s="38"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
-      <c r="F123" s="39"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="40"/>
+      <c r="E123" s="40"/>
+      <c r="F123" s="40"/>
       <c r="G123" s="36"/>
     </row>
     <row r="124" ht="15.5" customHeight="1">
-      <c r="A124" s="38"/>
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="39"/>
-      <c r="F124" s="39"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
+      <c r="E124" s="40"/>
+      <c r="F124" s="40"/>
       <c r="G124" s="36"/>
     </row>
     <row r="125" ht="15.5" customHeight="1">

</xml_diff>